<commit_message>
feat: Implementar edición de oraciones y botones de navegación en tablas de tiempos verbales
</commit_message>
<xml_diff>
--- a/public/estructura.xlsx
+++ b/public/estructura.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Documents\PORTAFOLIO\grammanual\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="598"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,23 +19,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="167">
   <si>
     <t>TIEMPO</t>
   </si>
@@ -121,21 +110,12 @@
     <t>PRONOMBRE + VERBO LEXICO EN PASADO + NOT+ COMPLEMENTO ORACION</t>
   </si>
   <si>
-    <t>ELLA CORRIA POR EL BOSQUE</t>
-  </si>
-  <si>
     <t>VERBO AUXILIAR "DID" + PRONOMBRE + VERBO LEXICO EN PRESENTE + C.O</t>
   </si>
   <si>
     <t>VERBO AUXILIAR "DID" + NOT +  PRONOMBRE + VERBO LEXICO EN PRESENTE + C.O</t>
   </si>
   <si>
-    <t>SHE RAN FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>HE DID NOT RUN FOR THE FOREST</t>
-  </si>
-  <si>
     <t>FUTURO 1ER CONDICIONAL</t>
   </si>
   <si>
@@ -148,48 +128,9 @@
     <t>PRONOMBRE + VERBO AUXILIAR  DID + NOT + VERBO LEXICO EN PRESENTE SIMPLE+ C.O</t>
   </si>
   <si>
-    <t>THEY WENT FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>WE DID NOT GO FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>DID SHE RUN FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t>DID NOT HE RUN FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t>DID I RUN FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t>DID NOT SHE RUN FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>SHE HAD RUN FOR THE FOREST</t>
-  </si>
-  <si>
     <t>PRONOMBRE + VERBO LEXICO EN PASADO SIMPLE  + COMPLEMENTO ORACION   (C.O)</t>
   </si>
   <si>
-    <t>SHE HAD NOT RUN FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>WE HAD NOT RUN FOT THE FOREST</t>
-  </si>
-  <si>
-    <t>HAD SHE RUN FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t>HAD NOT SHE RUN FOR THE FOREST?</t>
-  </si>
-  <si>
-    <t>HAD THEY RUN FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAD NOT YOU RUN FOR THE FOREST ? </t>
-  </si>
-  <si>
     <t>VERBO AUXILIAR "HAD" + NOT +  PRONOMBRE + VERBO LEXICO EN PRESENTE + C.O</t>
   </si>
   <si>
@@ -208,36 +149,12 @@
     <t xml:space="preserve">NOSOTROS NO CORRIMOS POR EL BOSQUE </t>
   </si>
   <si>
-    <t xml:space="preserve">TRADUCCION ALTERNATIVA </t>
-  </si>
-  <si>
-    <t>¿ YO CORRIA POR EL BOSQUE ?</t>
-  </si>
-  <si>
-    <t>¿ ELLA NO CORRIA POR EL BOSQUE?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿ ÉL NO CORRIA POR EL BOSQUE ? </t>
-  </si>
-  <si>
-    <t>¿ ELLA CORRIA POR EL BOSQUE ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOSOTROS NO CORRIAMOS POR EL BOSQUE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELLOS CORRIAN POR EL BOSQUE </t>
-  </si>
-  <si>
     <t>ELLA CORRIÓ POR EL BOSQUE</t>
   </si>
   <si>
     <t>ÉL NO CORRIÓ POR EL BOSQUE</t>
   </si>
   <si>
-    <t xml:space="preserve">ÉL NO CORRIA POR EL BOSQUE </t>
-  </si>
-  <si>
     <t>¿ ELLA CORRIÓ POR EL BOSQUE ?</t>
   </si>
   <si>
@@ -256,9 +173,6 @@
     <t>ELLA NO HABIA CORRIDO POR EL BOSQUE</t>
   </si>
   <si>
-    <t>THEY HAD RUN FOR THE FOREST</t>
-  </si>
-  <si>
     <t xml:space="preserve">ELLOS HABIAN CORRIDO POR EL BOSQUE </t>
   </si>
   <si>
@@ -268,78 +182,18 @@
     <t>¿ HABIA ELLA CORRIDO POR EL BOSQUE  ?</t>
   </si>
   <si>
-    <t>¿  HABIA CORRIDO ELLA POR EL BOSQUE ?</t>
-  </si>
-  <si>
     <t>¿ NO HABIA ELLA CORRIDO POR EL BOSQUE  ?</t>
   </si>
   <si>
-    <t>¿ NO HABIA CORRIDO ELLA POR EL BOSQUE  ?</t>
-  </si>
-  <si>
     <t>¿ HABIAN ELLOS CORRIDO POR EL BOSQUE ?</t>
   </si>
   <si>
-    <t>¿ HABIAN CORRIDO ELLOS AL BOSQUE ?</t>
-  </si>
-  <si>
     <t>¿  NO HABIAS TU CORRIDO POR EL BOSQUE ?</t>
   </si>
   <si>
-    <t>¿ NO HABIAS CORRIDO TU POR EL BOSQUE  ?</t>
-  </si>
-  <si>
-    <t>SHE WAS RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>SHE WAS NOT RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>THEY WERE RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>THEY WERE NOT RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>WAS SHE RUNNING FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAS NOT SHE RUNNING FOR THE FOREST ? </t>
-  </si>
-  <si>
     <t>WERE</t>
   </si>
   <si>
-    <t>WERE THEY RUNNNING FOR THE FORES T</t>
-  </si>
-  <si>
-    <t>WERE NOT THEY RUNNING FOR THE FOREST?</t>
-  </si>
-  <si>
-    <t>SHE HAD BEEN RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>SHE HAD BEEN NOT RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>WE HAD BEEN NOT RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>WE HAD BEEN RUNNING FOR THE FOREST</t>
-  </si>
-  <si>
-    <t>HAD BEEN SHE RUNNING FOR THE FOREST ?</t>
-  </si>
-  <si>
-    <t>HAD BEEN NOT RUNNING FOR THE FOREST?</t>
-  </si>
-  <si>
-    <t>HAD BEEN WE RUNNING FOR THE FOREST?</t>
-  </si>
-  <si>
-    <t>HAD BEEN NOT WE RUNNING FOR THE FOREST?</t>
-  </si>
-  <si>
     <t>SHE RUNS FOR THE FOREST</t>
   </si>
   <si>
@@ -436,12 +290,6 @@
     <t>HAVE BEEN THEY RUNNING FOR THE FOREST?</t>
   </si>
   <si>
-    <t>HAS NOT BEEN SHE RUNNING FOR THE FOREST?</t>
-  </si>
-  <si>
-    <t>HAVE BEEN NOT THE RUNNING FOR THE FOREST?</t>
-  </si>
-  <si>
     <t>PRONOMBRE+ VERBO AUXILIAR "WAS"+VERBO LEXICO EN PRESENTE SIMPLE  +ING +C.O</t>
   </si>
   <si>
@@ -551,13 +399,139 @@
   </si>
   <si>
     <t>VERBO AUXILIAR "TOBE( ARE)"+NOT+PRONOMBRE+VERBO LEXICO EN PRESENTE+ING+C.O?</t>
+  </si>
+  <si>
+    <t>SHE RAN INTO THE FOREST</t>
+  </si>
+  <si>
+    <t>DID SHE RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>DID HE NOT RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>DID I RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>DID SHE NOT RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>SHE HAD RUN TO THE FOREST</t>
+  </si>
+  <si>
+    <t>SHE HAD NOT RUN TO THE FOREST</t>
+  </si>
+  <si>
+    <t>THEY HAD RUN TO THE FOREST</t>
+  </si>
+  <si>
+    <t>WE HAD NOT RUN TO THE FOREST</t>
+  </si>
+  <si>
+    <t>HAD SHE RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAD SHE NOT RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAD THEY RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAD YOU NOT RUN TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>SHE WAS RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>SHE WAS NOT RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>THEY WERE RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>THEY WERE NOT RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>WAS SHE RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>WAS SHE NOT RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>WERE THEY RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>WERE THEY NOT RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>SHE HAD BEEN RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>SHE HAD NOT BEEN RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>WE HAD BEEN RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>WE HAD NOT BEEN RUNNING TO THE FOREST</t>
+  </si>
+  <si>
+    <t>HAD SHE BEEN RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAD SHE NOT BEEN RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAD WE BEEN RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAD WE NOT BEEN RUNNING TO THE FOREST?</t>
+  </si>
+  <si>
+    <t>PRONOMBRE+VERBO AUXILIAR "HAVE"+VERBO AUXILIAR "TOBE (BEEN) "+ NOT+ VERBO LEXICO EN PRESENTE+ING+C.O</t>
+  </si>
+  <si>
+    <t>PRONOMBRE+VERBO AUXILIAR "HAVE"+VERBO AUXILIAR "TOBE (BEEN) " + VERBO LEXICO EN PRESENTE+ING+C.O</t>
+  </si>
+  <si>
+    <t>VERBO AUXILIAR "HAVE" + VERBO AUXILIAR "TOBE( BEEN)" + PRONOMBRE+VERBO LEXICO EN PRESENTE+ING+C.O?</t>
+  </si>
+  <si>
+    <t>PRONOMBRE+VERBO AUXILIAR "HAS"+VERBO AUXILIAR "TOBE (BEEN) "+VERBO LEXICO EN PRESENTE+ING+C.O</t>
+  </si>
+  <si>
+    <t>PRONOMBRE+VERBO AUXILIAR "HAS"+VERBO AUXILIAR "TOBE (BEEN) "+ NOT+ VERBO LEXICO EN PRESENTE+ING+C.O</t>
+  </si>
+  <si>
+    <t>VERBO AUXILIAR "HAS" + VERBO AUXILIAR "TOBE( BEEN)" + PRONOMBRE+VERBO LEXICO EN PRESENTE+ING+C.O?</t>
+  </si>
+  <si>
+    <t>HAVE BEEN NOT THEY RUNNING FOR THE FOREST?</t>
+  </si>
+  <si>
+    <t>HAS  BEEN NOT SHE RUNNING FOR THE FOREST?</t>
+  </si>
+  <si>
+    <t>VERBO AUXILIAR "HAS" + VERBO AUXILIAR "TOBE( BEEN)" + NOT +  PRONOMBRE+VERBO LEXICO EN PRESENTE+ING+C.O?</t>
+  </si>
+  <si>
+    <t>VERBO AUXILIAR "HAVE" + VERBO AUXILIAR "TOBE( BEEN)" + NOT +  PRONOMBRE+VERBO LEXICO EN PRESENTE+ING+C.O?</t>
+  </si>
+  <si>
+    <t>HE DID NOT RUN INTO THE FOREST</t>
+  </si>
+  <si>
+    <t>WE DID NOT RUN INTO THE FOREST</t>
+  </si>
+  <si>
+    <t>THEY RAN INTO THE FOREST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,8 +546,16 @@
       <name val="Aharoni"/>
       <charset val="177"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +586,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -617,13 +605,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,25 +900,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD99"/>
+  <dimension ref="A1:XFC99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8" style="4" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="98" style="1" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="52.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="40" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62" style="1" customWidth="1"/>
+    <col min="5" max="5" width="53.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.3984375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -947,11 +936,8 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -962,19 +948,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -985,19 +968,16 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1008,19 +988,16 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1033,17 +1010,14 @@
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
+      <c r="E5" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1054,19 +1028,16 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1077,19 +1048,16 @@
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1100,19 +1068,16 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1123,19 +1088,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1146,19 +1108,16 @@
         <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -1169,19 +1128,16 @@
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
@@ -1192,19 +1148,16 @@
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1215,19 +1168,16 @@
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1238,19 +1188,16 @@
         <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1261,19 +1208,16 @@
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1284,19 +1228,16 @@
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7 16384:16384">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6 16383:16383" ht="18">
       <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
@@ -1307,19 +1248,16 @@
         <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7 16384:16384">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6 16383:16383" ht="18">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -1330,16 +1268,16 @@
         <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7 16384:16384">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6 16383:16383" ht="18">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -1350,16 +1288,16 @@
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7 16384:16384">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6 16383:16383" ht="18">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1370,13 +1308,13 @@
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7 16384:16384">
+        <v>90</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6 16383:16383" ht="18">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1387,13 +1325,13 @@
         <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7 16384:16384">
+        <v>91</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6 16383:16383" ht="18">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
@@ -1404,13 +1342,13 @@
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7 16384:16384">
+        <v>92</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6 16383:16383" ht="18">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -1421,13 +1359,13 @@
         <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7 16384:16384">
+        <v>93</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6 16383:16383" ht="18">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1438,16 +1376,16 @@
         <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="XFD24" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7 16384:16384">
+        <v>94</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="XFC24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6 16383:16383" ht="18">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
@@ -1458,13 +1396,13 @@
         <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7 16384:16384">
+        <v>95</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6 16383:16383" ht="18">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -1475,13 +1413,13 @@
         <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7 16384:16384">
+        <v>96</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6 16383:16383" ht="18">
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
@@ -1492,13 +1430,13 @@
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7 16384:16384">
+        <v>97</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6 16383:16383" ht="18">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -1509,13 +1447,13 @@
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7 16384:16384">
+        <v>98</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6 16383:16383" ht="18">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1526,13 +1464,13 @@
         <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7 16384:16384">
+        <v>98</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6 16383:16383" ht="18">
       <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
@@ -1543,13 +1481,13 @@
         <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7 16384:16384">
+        <v>105</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6 16383:16383" ht="18">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
@@ -1560,13 +1498,13 @@
         <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7 16384:16384">
+    </row>
+    <row r="32" spans="1:6 16383:16383" ht="18">
       <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
@@ -1577,13 +1515,13 @@
         <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>104</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
@@ -1594,10 +1532,10 @@
         <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1">
@@ -1614,10 +1552,10 @@
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1631,10 +1569,10 @@
         <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1648,10 +1586,10 @@
         <v>13</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1665,10 +1603,10 @@
         <v>14</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1682,10 +1620,10 @@
         <v>15</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1699,10 +1637,10 @@
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1716,10 +1654,10 @@
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1733,10 +1671,10 @@
         <v>18</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1750,10 +1688,10 @@
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1767,10 +1705,10 @@
         <v>12</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1784,10 +1722,10 @@
         <v>13</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1801,10 +1739,10 @@
         <v>14</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1818,10 +1756,10 @@
         <v>15</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1835,10 +1773,10 @@
         <v>16</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1852,10 +1790,10 @@
         <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1869,10 +1807,10 @@
         <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1886,10 +1824,10 @@
         <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1903,10 +1841,10 @@
         <v>12</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1920,10 +1858,10 @@
         <v>13</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1937,10 +1875,10 @@
         <v>14</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1954,10 +1892,10 @@
         <v>15</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1971,10 +1909,10 @@
         <v>16</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1988,10 +1926,10 @@
         <v>17</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2005,122 +1943,146 @@
         <v>18</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="D59" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="E59" s="1" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="D60" s="6" t="s">
+        <v>158</v>
+      </c>
       <c r="E60" s="1" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D61" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="E61" s="1" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="D62" s="6" t="s">
+        <v>154</v>
+      </c>
       <c r="E62" s="1" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="D63" s="6" t="s">
+        <v>159</v>
+      </c>
       <c r="E63" s="1" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="D64" s="6" t="s">
+        <v>162</v>
+      </c>
       <c r="E64" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="D65" s="6" t="s">
+        <v>156</v>
+      </c>
       <c r="E65" s="1" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="D66" s="6" t="s">
+        <v>163</v>
+      </c>
       <c r="E66" s="1" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1">
@@ -2307,7 +2269,7 @@
         <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>11</v>
@@ -2318,7 +2280,7 @@
         <v>24</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>12</v>
@@ -2329,7 +2291,7 @@
         <v>24</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>13</v>
@@ -2340,7 +2302,7 @@
         <v>24</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>14</v>
@@ -2351,7 +2313,7 @@
         <v>24</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>15</v>
@@ -2362,7 +2324,7 @@
         <v>24</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>16</v>
@@ -2373,7 +2335,7 @@
         <v>24</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>17</v>
@@ -2384,7 +2346,7 @@
         <v>24</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>18</v>
@@ -2395,7 +2357,7 @@
         <v>24</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>11</v>
@@ -2406,7 +2368,7 @@
         <v>24</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>12</v>
@@ -2417,7 +2379,7 @@
         <v>24</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>13</v>
@@ -2428,7 +2390,7 @@
         <v>24</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>14</v>
@@ -2439,7 +2401,7 @@
         <v>24</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>15</v>
@@ -2450,7 +2412,7 @@
         <v>24</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>16</v>
@@ -2461,7 +2423,7 @@
         <v>24</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>17</v>
@@ -2472,7 +2434,7 @@
         <v>24</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>18</v>
@@ -2480,5 +2442,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>